<commit_message>
Update Journal_de_travail_VMW.xlsx Ajout de la classe Quiz
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail_VMW.xlsx
+++ b/Documentation/Journal_de_travail_VMW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63nch\Documents\GitHub\JoQuiz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63nch\Documents\GitHub\JoQuiz\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE2059D-EB1A-46E9-A5CF-EE0B56F2BD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA48DF6F-900F-474C-BB4C-BCF2A28F63BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14340" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Erreur dans le cahier des charge signalée a monsieur Savary</t>
   </si>
   <si>
-    <t>Rendez vous avec monsieur Savari</t>
-  </si>
-  <si>
     <t>Planification du projet</t>
   </si>
   <si>
@@ -111,13 +108,61 @@
     <t>Correction des objectifs</t>
   </si>
   <si>
-    <t>Discution a propos d'administratif avec monsieur Altieri</t>
-  </si>
-  <si>
     <t>Discution a propos d'un changement d'horaire avec monsieur Altieri</t>
   </si>
   <si>
-    <t>s</t>
+    <t>Programmation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Programmation</t>
+  </si>
+  <si>
+    <t>Instatalation IDE et emulateur</t>
+  </si>
+  <si>
+    <t>Création du projet sur android studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des autres layout </t>
+  </si>
+  <si>
+    <t>Ajout de boutons pour naviguer entre les differents layouts</t>
+  </si>
+  <si>
+    <t>Prise en main de L'IDE et test des differentes fonctions</t>
+  </si>
+  <si>
+    <t>Kendra Crystalle Gueissaz</t>
+  </si>
+  <si>
+    <t>Rendez vous avec monsieur Savary</t>
+  </si>
+  <si>
+    <t>J'ai consulté cette video qui m'a beaucoup aidé dans les premiers pas avec Kotlin et android studio https://youtu.be/BBWyXo-3JGQ?si=mxnYdjO_-LIGIdVp</t>
+  </si>
+  <si>
+    <t>J'ai d'abord essayé de faire une liste de bouton pour le menu principal et n'a pas réussi par manque de connaissance a propos des adaptateur</t>
+  </si>
+  <si>
+    <t>Developement du premier layout (menu principal)</t>
+  </si>
+  <si>
+    <t>Je n'avais pas compris qu'il fallait que j'ajoute les autres classes et layout egualement dans le androidmanifest.xml ce qui m'a beaucoup bloqué</t>
+  </si>
+  <si>
+    <t>Recherche sur les differentes façon d'organiser mon code</t>
+  </si>
+  <si>
+    <t>J'ai essayer de demander a chat gpt des information la dessus mais il n'est capable que de me montrer des exemples de code directement dans la main class ou inventer des dossier qui n'existent pas sans vraiment de sens</t>
+  </si>
+  <si>
+    <t>15h20</t>
+  </si>
+  <si>
+    <t>Journal de travail et mise en ordre github</t>
+  </si>
+  <si>
+    <t>Discussion a propos d'administratif avec monsieur Altieri</t>
   </si>
 </sst>
 </file>
@@ -539,7 +584,7 @@
   <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +595,7 @@
     <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="93.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,7 +711,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7">
@@ -693,7 +739,9 @@
       <c r="F7" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -763,7 +811,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="7">
         <v>0.40972222222222227</v>
@@ -781,7 +829,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7">
@@ -803,7 +851,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="7">
         <v>0.63888888888888895</v>
@@ -821,7 +869,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7">
@@ -840,7 +888,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7">
@@ -852,8 +900,8 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
+      <c r="A16" s="3">
+        <v>45331</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -871,75 +919,163 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="3">
+        <v>45331</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.59375</v>
+      </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>45342</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
+      <c r="E18" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>45342</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45342</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45342</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="3">
+        <v>45344</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>45344</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="3">
+        <v>45344</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1318,22 +1454,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A44E17421B74B4385ED2944255AEAB1" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="ec1f11910d9d3d31f415dc33befb08f2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad8f3c216865d387afcb6cef8ca7fe1b">
     <xsd:element name="properties">
@@ -1447,6 +1575,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1454,14 +1591,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1869183-61D9-4DD2-9578-8215B01A00EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1473,6 +1602,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Mise a jour documentation
Diagramme
Journal de travail et dossier de projet
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail_VMW.xlsx
+++ b/Documentation/Journal_de_travail_VMW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63nch\Documents\GitHub\JoQuiz\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA48DF6F-900F-474C-BB4C-BCF2A28F63BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71100405-7C28-42A4-B263-FA67332CA394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Developement du premier layout (menu principal)</t>
   </si>
   <si>
-    <t>Je n'avais pas compris qu'il fallait que j'ajoute les autres classes et layout egualement dans le androidmanifest.xml ce qui m'a beaucoup bloqué</t>
-  </si>
-  <si>
     <t>Recherche sur les differentes façon d'organiser mon code</t>
   </si>
   <si>
@@ -163,6 +160,66 @@
   </si>
   <si>
     <t>Discussion a propos d'administratif avec monsieur Altieri</t>
+  </si>
+  <si>
+    <t>Je n'avais pas compris qu'il fallait que j'ajoute les autres classes et layout égualement dans le androidmanifest.xml ce qui m'a beaucoup bloqué</t>
+  </si>
+  <si>
+    <t>Commentaire du code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autre </t>
+  </si>
+  <si>
+    <t>Correction de details dans la documentation</t>
+  </si>
+  <si>
+    <t>Apprentissage de comment fonctionne les adaptateur sur kotlin</t>
+  </si>
+  <si>
+    <t>J'ai consulté cette video comme point de depart https://youtu.be/BBWyXo-3JGQ?si=mxnYdjO_-LIGIdVp</t>
+  </si>
+  <si>
+    <t>Création du layout pour un menu de bouton déroulant</t>
+  </si>
+  <si>
+    <t>Création de tout les fichiers necessaire au menu</t>
+  </si>
+  <si>
+    <t>j'ai adapté ce tutoriel a mon projet https://www.practicalcoding.net/post/recyclerview-item-click-kotlin</t>
+  </si>
+  <si>
+    <t>Bug les donnée ne sont pas affiché dans le recycler view</t>
+  </si>
+  <si>
+    <t>Correction bug menu</t>
+  </si>
+  <si>
+    <t>Pas résolu, le problèmes viens de ma classe QuizRepository</t>
+  </si>
+  <si>
+    <t>Le menu fonctionne enfin, erreur -&gt; typo dans les noms, je prévois d'ordonner cette partie du code plus tard pour éviter la confusion</t>
+  </si>
+  <si>
+    <t>Essai d'ajout d'XML</t>
+  </si>
+  <si>
+    <t>Il faut que je me renseigne plus sur le sujet</t>
+  </si>
+  <si>
+    <t>Documentation conception projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal de travail </t>
+  </si>
+  <si>
+    <t>Diagramme de flux du point de vue utilisateur</t>
+  </si>
+  <si>
+    <t>Pour la conception</t>
+  </si>
+  <si>
+    <t>Documentation realisation</t>
   </si>
 </sst>
 </file>
@@ -172,10 +229,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,11 +261,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -221,6 +296,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -269,8 +347,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:G26" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G26" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:G37" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G37" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F03BD8AE-DCAD-435E-AC03-584E15FC8493}" name="Date" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{76FA6963-7F8C-4895-B8BA-445A4BB2DC8E}" name="Type de travail" dataDxfId="5"/>
@@ -583,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4812EB-3ED2-43D9-9F10-833A2D245EB4}">
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7">
@@ -1006,13 +1084,13 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F21" s="7">
         <v>0.70486111111111116</v>
@@ -1049,7 +1127,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E23" s="7">
         <v>0.40972222222222227</v>
@@ -1067,7 +1145,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7">
@@ -1079,108 +1157,307 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="3">
+        <v>45344</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="3">
+        <v>45344</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>45345</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>45345</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.59375</v>
+      </c>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>45349</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>45349</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>45349</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>45349</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>45349</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>45351</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>45351</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>45351</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>45351</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
@@ -1462,6 +1739,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A44E17421B74B4385ED2944255AEAB1" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="ec1f11910d9d3d31f415dc33befb08f2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad8f3c216865d387afcb6cef8ca7fe1b">
     <xsd:element name="properties">
@@ -1575,15 +1861,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1591,6 +1868,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1869183-61D9-4DD2-9578-8215B01A00EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1602,14 +1887,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>